<commit_message>
FIX: Load test files with different locales (HACK)
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/T_VALUE_VALUETOTEXT.xlsx
+++ b/xlsx/tests/calc_tests/T_VALUE_VALUETOTEXT.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Dropbox/Excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857875EF-591A-F441-A66D-1D2822DE4D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FE4AAAF-499A-4C0E-A774-AFE93831C722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{90BFB5BF-1E97-AE4E-BD59-5D1CAC242620}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="1" xr2:uid="{90BFB5BF-1E97-AE4E-BD59-5D1CAC242620}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>value</t>
   </si>
@@ -44,55 +45,61 @@
     <t>T</t>
   </si>
   <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>VALUETOTEXT</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
     <t>123</t>
   </si>
   <si>
+    <t>23€</t>
+  </si>
+  <si>
+    <t>23.123%</t>
+  </si>
+  <si>
     <t>qwerty</t>
   </si>
   <si>
-    <t>VALUE</t>
-  </si>
-  <si>
-    <t>VALUETOTEXT</t>
+    <t>10-12-1999</t>
+  </si>
+  <si>
+    <t>40-2-2023</t>
+  </si>
+  <si>
+    <t>2-Feb-2026</t>
   </si>
   <si>
     <t>1e-5</t>
   </si>
   <si>
+    <t>30/2/2010</t>
+  </si>
+  <si>
+    <t>12€</t>
+  </si>
+  <si>
+    <t>123,456.67</t>
+  </si>
+  <si>
+    <t>12,34</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>2/3/2023</t>
   </si>
   <si>
-    <t>40%</t>
-  </si>
-  <si>
-    <t>23€</t>
-  </si>
-  <si>
-    <t>23.123%</t>
-  </si>
-  <si>
-    <t>10-12-1999</t>
-  </si>
-  <si>
-    <t>40-2-2023</t>
-  </si>
-  <si>
-    <t>2-Feb-2026</t>
-  </si>
-  <si>
-    <t>30/2/2010</t>
-  </si>
-  <si>
-    <t>123,456.67</t>
-  </si>
-  <si>
-    <t>12,34</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>12€</t>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>en-GB</t>
   </si>
 </sst>
 </file>
@@ -100,9 +107,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -186,7 +193,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -506,17 +513,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8063A25-DCAC-6E43-B5F7-BE51B981F4AA}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -524,19 +531,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" s="3" t="str">
         <f>T(A2)</f>
         <v/>
@@ -550,16 +557,16 @@
         <v/>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I2" s="3">
         <f>VALUE(H2)</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="str">
         <f t="shared" ref="B3:B14" si="0">T(A3)</f>
@@ -574,14 +581,14 @@
         <v>123</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I20" si="3">VALUE(H3)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>123</v>
       </c>
@@ -598,16 +605,16 @@
         <v>123</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="3"/>
         <v>0.23122999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -622,14 +629,14 @@
         <v>qwerty</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="3"/>
         <v>36504</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -646,14 +653,14 @@
         <v>TRUE</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" s="3" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
@@ -671,16 +678,16 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="3"/>
         <v>46055</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ref="B8:B11" si="4">T(A8)</f>
@@ -695,16 +702,16 @@
         <v>1e-5</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="I8" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" si="4"/>
@@ -726,7 +733,7 @@
         <v>123456.67</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>1.2344999999999999</v>
       </c>
@@ -750,7 +757,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="2">
         <v>7.1234560000000001E-9</v>
       </c>
@@ -774,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="B12" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -795,7 +802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="2">
         <v>4200</v>
       </c>
@@ -820,7 +827,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -842,9 +849,9 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="str">
         <f t="shared" ref="B15" si="7">T(A15)</f>
@@ -866,13 +873,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="I16" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="8:9">
       <c r="H17" s="7">
         <v>38169</v>
       </c>
@@ -881,7 +888,7 @@
         <v>38169</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="8:9">
       <c r="H18" s="7">
         <v>20886</v>
       </c>
@@ -890,7 +897,7 @@
         <v>20886</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="8:9">
       <c r="H19" s="8">
         <v>1234.567</v>
       </c>
@@ -899,10 +906,33 @@
         <v>1234.567</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="8:9">
       <c r="I20" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E9E4BC-8558-4DB5-9F9A-9793F11B543E}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>